<commit_message>
last edit for article
</commit_message>
<xml_diff>
--- a/styled_model_finish_behavioral_edit.xlsx
+++ b/styled_model_finish_behavioral_edit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jofy/Documents/Projects/FIIT-PRIPOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8109D2E7-BC19-1E46-84EA-D2A5BC2E202A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6E1D1B-339F-AF4D-B84B-D6BF3711747D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
   <si>
     <t>Count features</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>Algoritmus</t>
+  </si>
+  <si>
+    <t>Počer atributov</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>Percentá</t>
   </si>
 </sst>
 </file>
@@ -423,19 +435,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -741,7 +753,7 @@
   <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12:Q23"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -769,8 +781,8 @@
         <v>4</v>
       </c>
       <c r="P1" s="37"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -951,16 +963,16 @@
       <c r="F10" s="4">
         <v>5364.6717665195474</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="42" t="s">
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="40" t="s">
         <v>27</v>
       </c>
     </row>
@@ -983,20 +995,20 @@
       <c r="F11" s="4">
         <v>5364.6717665195474</v>
       </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44" t="s">
+      <c r="J11" s="41"/>
+      <c r="K11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="44" t="s">
+      <c r="M11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="44" t="s">
+      <c r="N11" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="O11" s="43"/>
+      <c r="O11" s="41"/>
       <c r="Q11" t="s">
         <v>25</v>
       </c>
@@ -1020,27 +1032,27 @@
       <c r="F12" s="4">
         <v>5364.6717665195474</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="45">
+      <c r="K12" s="43">
         <v>0.54087291121828207</v>
       </c>
-      <c r="L12" s="45">
+      <c r="L12" s="43">
         <v>0.55068550387301096</v>
       </c>
-      <c r="M12" s="45">
+      <c r="M12" s="43">
         <v>0.54059513344050436</v>
       </c>
-      <c r="N12" s="45">
+      <c r="N12" s="43">
         <v>0.54087291121828207</v>
       </c>
-      <c r="O12" s="44" t="str">
+      <c r="O12" s="42" t="str">
         <f t="shared" ref="O12:O23" si="0">IF(K12=MAX(K12,L12,M12,N12),"GA",IF(L12=MAX(L12,M12,N12),"VIF",IF(M12=MAX(M12,N12),"CORR","Bez vyberu")))</f>
         <v>VIF</v>
       </c>
       <c r="Q12" s="38">
-        <f>K12-MAX(L12,M12,N12)</f>
+        <f t="shared" ref="Q12:Q23" si="1">K12-MAX(L12,M12,N12)</f>
         <v>-9.8125926547288911E-3</v>
       </c>
     </row>
@@ -1063,27 +1075,27 @@
       <c r="F13" s="4">
         <v>5364.6717665195474</v>
       </c>
-      <c r="J13" s="44" t="s">
+      <c r="J13" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="45">
+      <c r="K13" s="43">
         <v>0.84313449741082702</v>
       </c>
-      <c r="L13" s="45">
+      <c r="L13" s="43">
         <v>0.84864356665514928</v>
       </c>
-      <c r="M13" s="45">
+      <c r="M13" s="43">
         <v>0.83508198501420294</v>
       </c>
-      <c r="N13" s="45">
+      <c r="N13" s="43">
         <v>0.85698447232097164</v>
       </c>
-      <c r="O13" s="44" t="str">
+      <c r="O13" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Bez vyberu</v>
       </c>
       <c r="Q13" s="38">
-        <f>K13-MAX(L13,M13,N13)</f>
+        <f t="shared" si="1"/>
         <v>-1.3849974910144613E-2</v>
       </c>
     </row>
@@ -1106,27 +1118,27 @@
       <c r="F14" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="45">
+      <c r="K14" s="43">
         <v>0.76554473858844307</v>
       </c>
-      <c r="L14" s="45">
+      <c r="L14" s="43">
         <v>0.69790295138412572</v>
       </c>
-      <c r="M14" s="45">
+      <c r="M14" s="43">
         <v>0.68279849377123014</v>
       </c>
-      <c r="N14" s="45">
+      <c r="N14" s="43">
         <v>0.7547902968290563</v>
       </c>
-      <c r="O14" s="44" t="str">
+      <c r="O14" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q14" s="38">
-        <f>K14-MAX(L14,M14,N14)</f>
+        <f t="shared" si="1"/>
         <v>1.0754441759386779E-2</v>
       </c>
     </row>
@@ -1149,27 +1161,27 @@
       <c r="F15" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="45">
+      <c r="K15" s="43">
         <v>0.79187256536335715</v>
       </c>
-      <c r="L15" s="45">
+      <c r="L15" s="43">
         <v>0.86534335058210521</v>
       </c>
-      <c r="M15" s="45">
+      <c r="M15" s="43">
         <v>0.81349489283648091</v>
       </c>
-      <c r="N15" s="45">
+      <c r="N15" s="43">
         <v>0.79680219708716615</v>
       </c>
-      <c r="O15" s="44" t="str">
+      <c r="O15" s="42" t="str">
         <f t="shared" si="0"/>
         <v>VIF</v>
       </c>
       <c r="Q15" s="38">
-        <f>K15-MAX(L15,M15,N15)</f>
+        <f t="shared" si="1"/>
         <v>-7.3470785218748058E-2</v>
       </c>
     </row>
@@ -1192,27 +1204,27 @@
       <c r="F16" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J16" s="44" t="s">
+      <c r="J16" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="45">
+      <c r="K16" s="43">
         <v>0.91523453978028912</v>
       </c>
-      <c r="L16" s="45">
+      <c r="L16" s="43">
         <v>0.13824074036114881</v>
       </c>
-      <c r="M16" s="45">
+      <c r="M16" s="43">
         <v>0.13824074036114881</v>
       </c>
-      <c r="N16" s="45">
+      <c r="N16" s="43">
         <v>0.13824074036114881</v>
       </c>
-      <c r="O16" s="44" t="str">
+      <c r="O16" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q16" s="38">
-        <f>K16-MAX(L16,M16,N16)</f>
+        <f t="shared" si="1"/>
         <v>0.77699379941914026</v>
       </c>
     </row>
@@ -1235,27 +1247,27 @@
       <c r="F17" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="K17" s="45">
+      <c r="K17" s="43">
         <v>0.94961898099691788</v>
       </c>
-      <c r="L17" s="45">
+      <c r="L17" s="43">
         <v>0.94745113259647895</v>
       </c>
-      <c r="M17" s="45">
+      <c r="M17" s="43">
         <v>0.9379646528768294</v>
       </c>
-      <c r="N17" s="45">
+      <c r="N17" s="43">
         <v>0.96125138935009302</v>
       </c>
-      <c r="O17" s="44" t="str">
+      <c r="O17" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Bez vyberu</v>
       </c>
       <c r="Q17" s="38">
-        <f>K17-MAX(L17,M17,N17)</f>
+        <f t="shared" si="1"/>
         <v>-1.1632408353175139E-2</v>
       </c>
     </row>
@@ -1278,27 +1290,27 @@
       <c r="F18" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J18" s="44" t="s">
+      <c r="J18" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K18" s="43">
         <v>0.95237619712914301</v>
       </c>
-      <c r="L18" s="45">
+      <c r="L18" s="43">
         <v>0.95656363970638092</v>
       </c>
-      <c r="M18" s="45">
+      <c r="M18" s="43">
         <v>0.94575388419730844</v>
       </c>
-      <c r="N18" s="45">
+      <c r="N18" s="43">
         <v>0.95737008383105715</v>
       </c>
-      <c r="O18" s="44" t="str">
+      <c r="O18" s="42" t="str">
         <f t="shared" si="0"/>
         <v>Bez vyberu</v>
       </c>
       <c r="Q18" s="38">
-        <f>K18-MAX(L18,M18,N18)</f>
+        <f t="shared" si="1"/>
         <v>-4.9938867019141409E-3</v>
       </c>
     </row>
@@ -1321,27 +1333,27 @@
       <c r="F19" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="45">
+      <c r="K19" s="43">
         <v>0.9390870654602933</v>
       </c>
-      <c r="L19" s="45">
+      <c r="L19" s="43">
         <v>0.71261093295404032</v>
       </c>
-      <c r="M19" s="45">
+      <c r="M19" s="43">
         <v>0.6927773611610859</v>
       </c>
-      <c r="N19" s="45">
+      <c r="N19" s="43">
         <v>0.7638141070686677</v>
       </c>
-      <c r="O19" s="44" t="str">
+      <c r="O19" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q19" s="38">
-        <f>K19-MAX(L19,M19,N19)</f>
+        <f t="shared" si="1"/>
         <v>0.1752729583916256</v>
       </c>
     </row>
@@ -1364,27 +1376,27 @@
       <c r="F20" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="J20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="45">
+      <c r="K20" s="43">
         <v>0.73063492856880818</v>
       </c>
-      <c r="L20" s="45">
+      <c r="L20" s="43">
         <v>0.69528350468052547</v>
       </c>
-      <c r="M20" s="45">
+      <c r="M20" s="43">
         <v>0.69642635075348225</v>
       </c>
-      <c r="N20" s="45">
+      <c r="N20" s="43">
         <v>0.6871515532216611</v>
       </c>
-      <c r="O20" s="44" t="str">
+      <c r="O20" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q20" s="38">
-        <f>K20-MAX(L20,M20,N20)</f>
+        <f t="shared" si="1"/>
         <v>3.4208577815325936E-2</v>
       </c>
     </row>
@@ -1407,27 +1419,27 @@
       <c r="F21" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="45">
+      <c r="K21" s="43">
         <v>0.1892526826838791</v>
       </c>
-      <c r="L21" s="45">
+      <c r="L21" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="M21" s="45">
+      <c r="M21" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="N21" s="45">
+      <c r="N21" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="O21" s="44" t="str">
+      <c r="O21" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q21" s="38">
-        <f>K21-MAX(L21,M21,N21)</f>
+        <f t="shared" si="1"/>
         <v>5.5555555555558689E-4</v>
       </c>
     </row>
@@ -1450,27 +1462,27 @@
       <c r="F22" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="45">
+      <c r="K22" s="43">
         <v>0.2092092672125852</v>
       </c>
-      <c r="L22" s="45">
+      <c r="L22" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="M22" s="45">
+      <c r="M22" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="N22" s="45">
+      <c r="N22" s="43">
         <v>0.18869712712832351</v>
       </c>
-      <c r="O22" s="44" t="str">
+      <c r="O22" s="42" t="str">
         <f t="shared" si="0"/>
         <v>GA</v>
       </c>
       <c r="Q22" s="38">
-        <f>K22-MAX(L22,M22,N22)</f>
+        <f t="shared" si="1"/>
         <v>2.0512140084261693E-2</v>
       </c>
     </row>
@@ -1493,27 +1505,27 @@
       <c r="F23" s="18">
         <v>71266.492980480194</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="45">
+      <c r="K23" s="43">
         <v>0.86789294575086529</v>
       </c>
-      <c r="L23" s="45">
+      <c r="L23" s="43">
         <v>0.91381962391110716</v>
       </c>
-      <c r="M23" s="45">
+      <c r="M23" s="43">
         <v>0.86706043522673881</v>
       </c>
-      <c r="N23" s="45">
+      <c r="N23" s="43">
         <v>0.57358134955987017</v>
       </c>
-      <c r="O23" s="44" t="str">
+      <c r="O23" s="42" t="str">
         <f t="shared" si="0"/>
         <v>VIF</v>
       </c>
       <c r="Q23" s="38">
-        <f>K23-MAX(L23,M23,N23)</f>
+        <f t="shared" si="1"/>
         <v>-4.5926678160241874E-2</v>
       </c>
     </row>
@@ -1596,6 +1608,21 @@
       <c r="F27" s="16">
         <v>2.402950763702393</v>
       </c>
+      <c r="I27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1616,6 +1643,21 @@
       <c r="F28" s="16">
         <v>2.402950763702393</v>
       </c>
+      <c r="I28" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="2">
+        <v>260</v>
+      </c>
+      <c r="K28" s="16">
+        <v>190</v>
+      </c>
+      <c r="L28" s="25">
+        <v>255</v>
+      </c>
+      <c r="M28" s="18">
+        <v>562</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1696,8 +1738,23 @@
       <c r="F32" s="16">
         <v>2.402950763702393</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" t="s">
+        <v>22</v>
+      </c>
+      <c r="L32" t="s">
+        <v>23</v>
+      </c>
+      <c r="M32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1716,8 +1773,27 @@
       <c r="F33" s="16">
         <v>2.402950763702393</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="43">
+        <f>(J34/MAX($J$34,$K$34,$L$34,$M$34))*100</f>
+        <v>7.5276213858158094</v>
+      </c>
+      <c r="K33" s="43">
+        <f t="shared" ref="K33:M33" si="2">(K34/MAX($J$34,$K$34,$L$34,$M$34))*100</f>
+        <v>100</v>
+      </c>
+      <c r="L33" s="43">
+        <f t="shared" si="2"/>
+        <v>3.3717819738380539E-3</v>
+      </c>
+      <c r="M33" s="43">
+        <f t="shared" si="2"/>
+        <v>1.2658853042053027E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1736,8 +1812,27 @@
       <c r="F34" s="16">
         <v>2.402950763702393</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="43">
+        <v>5364.6717665195501</v>
+      </c>
+      <c r="K34" s="43">
+        <v>71266.492980480194</v>
+      </c>
+      <c r="L34" s="43">
+        <v>2.402950763702393</v>
+      </c>
+      <c r="M34" s="43">
+        <v>9.0215206146240234E-3</v>
+      </c>
+      <c r="P34">
+        <f>K34/J34</f>
+        <v>13.284408829119458</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1757,7 +1852,7 @@
         <v>2.402950763702393</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1777,7 +1872,7 @@
         <v>2.402950763702393</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1796,8 +1891,20 @@
       <c r="F37" s="16">
         <v>2.402950763702393</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J37" s="43">
+        <v>5364.6717665195474</v>
+      </c>
+      <c r="K37" s="43">
+        <v>71266.492980480194</v>
+      </c>
+      <c r="L37" s="43">
+        <v>2.402950763702393</v>
+      </c>
+      <c r="M37" s="43">
+        <v>9.0215206146240234E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1817,7 +1924,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1837,7 +1944,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1857,7 +1964,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1877,7 +1984,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1897,7 +2004,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1917,7 +2024,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1937,7 +2044,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1957,7 +2064,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1977,7 +2084,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1997,7 +2104,7 @@
         <v>9.0215206146240234E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>

</xml_diff>